<commit_message>
Adding book images and mappings along with updating API
</commit_message>
<xml_diff>
--- a/other/Sprint Books.xlsx
+++ b/other/Sprint Books.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11869626e8181b65/Documents/Colorado Technical University/CS492/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11869626e8181b65/Documents/Colorado Technical University/CS492/Bookstore/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_FFC65FC0CD81A8F2B849BB9D71746E8B6CD0D3CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E2DE67-F77A-420C-A1C1-E04BC0F1F012}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_FFC65FC0CD81A8F2B849BB9D71746E8B6CD0D3CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F875CAE1-AA35-4702-975A-944852952D1B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,6 +549,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,11 +845,15 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>

</xml_diff>